<commit_message>
Added new plots to RCode
</commit_message>
<xml_diff>
--- a/RCode/CovidSimAnalysis/deathData/NRSDeathsWK23.xlsx
+++ b/RCode/CovidSimAnalysis/deathData/NRSDeathsWK23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paul\Dropbox\Paul\Random\Covid\Simulation model\RCode\CovidSimAnalysis\deathData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFD17988-B7B5-4C35-877D-4D2E55919809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2957594E-410F-480B-95A8-C896D77B5E10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C7ECDD6D-129E-49C5-A7D2-7952AF1D6349}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C7ECDD6D-129E-49C5-A7D2-7952AF1D6349}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,11 +84,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="General_)"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +116,25 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="7.5"/>
+      <color indexed="12"/>
+      <name val="Helv"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -145,12 +165,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -162,11 +208,38 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="23">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="5" xr:uid="{9965AA7B-1553-4D14-B712-27A5AF446D4C}"/>
+    <cellStyle name="Comma 2 2" xfId="6" xr:uid="{A045EC9A-AFC7-4D31-A423-2ED2B6117C2F}"/>
+    <cellStyle name="Comma 3" xfId="7" xr:uid="{ECEECED7-8E5D-4AE8-B2F6-2F0B028D0800}"/>
+    <cellStyle name="Comma 3 2" xfId="8" xr:uid="{3E5FDC52-8601-43B3-806E-2CB601A2FAE2}"/>
+    <cellStyle name="Comma 4" xfId="9" xr:uid="{A66AA3E7-AF82-49AA-A879-8FFE477C4AFD}"/>
+    <cellStyle name="Comma 5" xfId="4" xr:uid="{8E46EE93-9D51-42C1-AB23-EEEAB251D4A9}"/>
+    <cellStyle name="Comma 6" xfId="20" xr:uid="{0378C6D1-DAC3-4CFC-9F85-90025D7CDCB2}"/>
+    <cellStyle name="Hyperlink 2" xfId="10" xr:uid="{6EC478B2-96EB-469D-A267-A6FEEE5956C0}"/>
+    <cellStyle name="Hyperlink 2 2" xfId="11" xr:uid="{0E90031A-F87E-4E48-A6F4-5EB1AC687AD8}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{51EB16BE-02F5-4702-AC6B-399B150D07B9}"/>
+    <cellStyle name="Normal 2 2" xfId="12" xr:uid="{F57F4C1E-7F46-45DB-8F04-879D76C569DE}"/>
+    <cellStyle name="Normal 2 2 2" xfId="13" xr:uid="{BD2F74DE-2A40-4B9A-BF92-9E21A23BC95A}"/>
+    <cellStyle name="Normal 2 3" xfId="14" xr:uid="{564D3B30-E767-4BAC-8CEA-CD0891AD0CF7}"/>
+    <cellStyle name="Normal 2 4" xfId="15" xr:uid="{82824FFA-0BE7-442F-B931-0D2F169E87B3}"/>
+    <cellStyle name="Normal 3" xfId="16" xr:uid="{AB2A733D-FC09-4D41-B477-5E41416FFA0C}"/>
+    <cellStyle name="Normal 3 2" xfId="17" xr:uid="{6EE81263-3B8F-4669-A0CB-65565A6ED5B9}"/>
+    <cellStyle name="Normal 3 3" xfId="18" xr:uid="{C4D567FC-65B2-43C1-92D0-A3F0E52104FE}"/>
+    <cellStyle name="Normal 4" xfId="19" xr:uid="{B39ED772-AA41-481C-AF08-C762B2ED8657}"/>
+    <cellStyle name="Normal 5" xfId="3" xr:uid="{D73AAE9B-4633-4A80-91E5-5F44A3CE8C88}"/>
+    <cellStyle name="Normal 6" xfId="21" xr:uid="{51CDD10B-E610-4320-8AA1-22F8DED14854}"/>
+    <cellStyle name="Percent 2" xfId="22" xr:uid="{90314BC2-A12C-455E-BD5E-C39C2C1C90E6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -478,13 +551,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C9ED1C-7414-4CD3-9A04-53C4C4939172}">
-  <dimension ref="A1:X15"/>
+  <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -557,8 +632,20 @@
       <c r="X1" s="4">
         <v>23</v>
       </c>
+      <c r="Y1" s="5">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="5">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="5">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="5">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,8 +718,20 @@
       <c r="X2" s="3">
         <v>6</v>
       </c>
+      <c r="Y2" s="7">
+        <v>6</v>
+      </c>
+      <c r="Z2" s="7">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -705,8 +804,20 @@
       <c r="X3" s="2">
         <v>6</v>
       </c>
+      <c r="Y3" s="6">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -779,8 +890,20 @@
       <c r="X4" s="2">
         <v>0</v>
       </c>
+      <c r="Y4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -853,8 +976,20 @@
       <c r="X5" s="2">
         <v>3</v>
       </c>
+      <c r="Y5" s="6">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="6">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -927,8 +1062,20 @@
       <c r="X6" s="2">
         <v>4</v>
       </c>
+      <c r="Y6" s="6">
+        <v>6</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>4</v>
+      </c>
+      <c r="AA6" s="6">
+        <v>3</v>
+      </c>
+      <c r="AB6" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1001,8 +1148,20 @@
       <c r="X7" s="2">
         <v>5</v>
       </c>
+      <c r="Y7" s="6">
+        <v>6</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>4</v>
+      </c>
+      <c r="AA7" s="6">
+        <v>3</v>
+      </c>
+      <c r="AB7" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1075,8 +1234,20 @@
       <c r="X8" s="2">
         <v>21</v>
       </c>
+      <c r="Y8" s="6">
+        <v>17</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>15</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>8</v>
+      </c>
+      <c r="AB8" s="6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1149,8 +1320,20 @@
       <c r="X9" s="2">
         <v>2</v>
       </c>
+      <c r="Y9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1223,8 +1406,20 @@
       <c r="X10" s="2">
         <v>18</v>
       </c>
+      <c r="Y10" s="6">
+        <v>8</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>8</v>
+      </c>
+      <c r="AA10" s="6">
+        <v>11</v>
+      </c>
+      <c r="AB10" s="6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1297,8 +1492,20 @@
       <c r="X11" s="2">
         <v>15</v>
       </c>
+      <c r="Y11" s="6">
+        <v>11</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>9</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>4</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1371,8 +1578,20 @@
       <c r="X12" s="2">
         <v>0</v>
       </c>
+      <c r="Y12" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1445,8 +1664,20 @@
       <c r="X13" s="2">
         <v>0</v>
       </c>
+      <c r="Y13" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1519,8 +1750,20 @@
       <c r="X14" s="2">
         <v>9</v>
       </c>
+      <c r="Y14" s="6">
+        <v>9</v>
+      </c>
+      <c r="Z14" s="6">
+        <v>2</v>
+      </c>
+      <c r="AA14" s="6">
+        <v>2</v>
+      </c>
+      <c r="AB14" s="6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1591,6 +1834,18 @@
         <v>0</v>
       </c>
       <c r="X15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>